<commit_message>
update CD1MR1 on park data
</commit_message>
<xml_diff>
--- a/scripts-in-progress/human-thymus/HumanThymus_22_ParkData_CD1dMR1/plots/flow_cytometry_plots/percentages.xlsx
+++ b/scripts-in-progress/human-thymus/HumanThymus_22_ParkData_CD1dMR1/plots/flow_cytometry_plots/percentages.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarcy/Projects/HumanThymusProject/scripts-in-progress/human-thymus/HumanThymus_22_ParkData_CD1dMR1/plots/flow_cytometry_plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D245CB58-21E1-5444-BCEB-4522535F3B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F7AF8-D936-C544-A7AD-A7E69B64A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16860" xr2:uid="{165F0C25-C340-1843-93F1-9DB2BDC1B7CA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16860" activeTab="1" xr2:uid="{165F0C25-C340-1843-93F1-9DB2BDC1B7CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="human" sheetId="1" r:id="rId1"/>
+    <sheet name="mouse" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$G$2:$G$27</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$E$2:$E$27</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$2:$H$27</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$D$27</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$2:$E$27</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$G$2:$G$27</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$H$2:$H$27</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$2:$D$27</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="37">
   <si>
     <t>sample</t>
   </si>
@@ -136,13 +123,37 @@
   </si>
   <si>
     <t>Northwell</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>CD45+</t>
+  </si>
+  <si>
+    <t>sample_age_weeks</t>
+  </si>
+  <si>
+    <t>wt1</t>
+  </si>
+  <si>
+    <t>wt2</t>
+  </si>
+  <si>
+    <t>wt3</t>
+  </si>
+  <si>
+    <t>rish</t>
+  </si>
+  <si>
+    <t>median_fluorescence_CD1d_pos_cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,6 +165,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,18 +207,192 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDD740F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF945200"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDD740F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF945200"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFDD740F"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF945200"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -572,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F5178A-3DDC-0347-B807-5578E1E396FB}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,23 +1481,364 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="mTEC">
+      <formula>NOT(ISERROR(SEARCH("mTEC",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="cTEC">
+      <formula>NOT(ISERROR(SEARCH("cTEC",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="CD8SP">
+      <formula>NOT(ISERROR(SEARCH("CD8SP",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="CD4SP">
+      <formula>NOT(ISERROR(SEARCH("CD4SP",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="DP">
+      <formula>NOT(ISERROR(SEARCH("DP",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="DN">
+      <formula>NOT(ISERROR(SEARCH("DN",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D76AAE-EAEE-B84F-9761-A4A29F52E7F0}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>6.3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45216</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>67</v>
+      </c>
+      <c r="H2">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>6.3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45216</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>6.3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45216</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>6.3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>6.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>64</v>
+      </c>
+      <c r="H6">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>6.3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>81</v>
+      </c>
+      <c r="H7">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>6.3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>61</v>
+      </c>
+      <c r="H8">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>6.3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>71</v>
+      </c>
+      <c r="H9">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>6.3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45233</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>94</v>
+      </c>
+      <c r="H10">
+        <v>494</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2:F3">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="mTEC">
+      <formula>NOT(ISERROR(SEARCH("mTEC",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="cTEC">
+      <formula>NOT(ISERROR(SEARCH("cTEC",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="CD8SP">
+      <formula>NOT(ISERROR(SEARCH("CD8SP",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="CD4SP">
+      <formula>NOT(ISERROR(SEARCH("CD4SP",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="DP">
+      <formula>NOT(ISERROR(SEARCH("DP",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="DN">
+      <formula>NOT(ISERROR(SEARCH("DN",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F6">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="mTEC">
+      <formula>NOT(ISERROR(SEARCH("mTEC",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="cTEC">
+      <formula>NOT(ISERROR(SEARCH("cTEC",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="CD8SP">
+      <formula>NOT(ISERROR(SEARCH("CD8SP",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="CD4SP">
+      <formula>NOT(ISERROR(SEARCH("CD4SP",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="DP">
+      <formula>NOT(ISERROR(SEARCH("DP",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="DN">
+      <formula>NOT(ISERROR(SEARCH("DN",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F9">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="mTEC">
-      <formula>NOT(ISERROR(SEARCH("mTEC",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("mTEC",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="cTEC">
-      <formula>NOT(ISERROR(SEARCH("cTEC",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("cTEC",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="CD8SP">
-      <formula>NOT(ISERROR(SEARCH("CD8SP",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("CD8SP",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="CD4SP">
-      <formula>NOT(ISERROR(SEARCH("CD4SP",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("CD4SP",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="DP">
-      <formula>NOT(ISERROR(SEARCH("DP",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DP",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="DN">
-      <formula>NOT(ISERROR(SEARCH("DN",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DN",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>